<commit_message>
Add pyarrow, update requirements
</commit_message>
<xml_diff>
--- a/tiempos_de_carga_29-01-2024.xlsx
+++ b/tiempos_de_carga_29-01-2024.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="19">
   <si>
     <t>Fecha</t>
   </si>
@@ -47,6 +47,18 @@
   </si>
   <si>
     <t>14:02:33</t>
+  </si>
+  <si>
+    <t>14:07:59</t>
+  </si>
+  <si>
+    <t>14:08:04</t>
+  </si>
+  <si>
+    <t>14:09:25</t>
+  </si>
+  <si>
+    <t>14:09:31</t>
   </si>
   <si>
     <t>registro_test_2</t>
@@ -416,7 +428,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -444,7 +456,7 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="D2">
         <v>2.34</v>
@@ -458,7 +470,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="D3">
         <v>5.2</v>
@@ -472,7 +484,7 @@
         <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="D4">
         <v>2.34</v>
@@ -486,7 +498,7 @@
         <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="D5">
         <v>5.26</v>
@@ -500,7 +512,7 @@
         <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="D6">
         <v>2.32</v>
@@ -514,10 +526,66 @@
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="D7">
         <v>5.18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8">
+        <v>2.33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9">
+        <v>5.24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10">
+        <v>2.34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11">
+        <v>5.2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add ejecutor (EJecutor de tareas en automatico)
</commit_message>
<xml_diff>
--- a/tiempos_de_carga_29-01-2024.xlsx
+++ b/tiempos_de_carga_29-01-2024.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="21">
   <si>
     <t>Fecha</t>
   </si>
@@ -59,6 +59,12 @@
   </si>
   <si>
     <t>14:09:31</t>
+  </si>
+  <si>
+    <t>17:12:09</t>
+  </si>
+  <si>
+    <t>17:12:15</t>
   </si>
   <si>
     <t>registro_test_2</t>
@@ -428,7 +434,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -456,7 +462,7 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D2">
         <v>2.34</v>
@@ -470,7 +476,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D3">
         <v>5.2</v>
@@ -484,7 +490,7 @@
         <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D4">
         <v>2.34</v>
@@ -498,7 +504,7 @@
         <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D5">
         <v>5.26</v>
@@ -512,7 +518,7 @@
         <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D6">
         <v>2.32</v>
@@ -526,7 +532,7 @@
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D7">
         <v>5.18</v>
@@ -540,7 +546,7 @@
         <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D8">
         <v>2.33</v>
@@ -554,7 +560,7 @@
         <v>12</v>
       </c>
       <c r="C9" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D9">
         <v>5.24</v>
@@ -568,7 +574,7 @@
         <v>13</v>
       </c>
       <c r="C10" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D10">
         <v>2.34</v>
@@ -582,10 +588,38 @@
         <v>14</v>
       </c>
       <c r="C11" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D11">
         <v>5.2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12">
+        <v>2.53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13">
+        <v>5.3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>